<commit_message>
performed eval for existing outputs
</commit_message>
<xml_diff>
--- a/output/Human Evaluation of Output.xlsx
+++ b/output/Human Evaluation of Output.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02a8352c8d6566ab/Documents/SMU MITB/CS605 NLP/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ef5aed61654d1d2/School/SMU/Modules/CS605_NLP_for_Smart_Assistants/Project/NLP-Lyric-Generator/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{3F379EBD-FB43-8A4D-A37E-DD25ED4CA8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C035A6D-F909-4C96-94A3-78815015C209}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{3F379EBD-FB43-8A4D-A37E-DD25ED4CA8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B60CFB2F-F5C6-420F-A94C-9C63F8A048BE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D62C98B2-5D28-40CA-95B7-0B218D23B21F}"/>
+    <workbookView xWindow="52455" yWindow="720" windowWidth="27045" windowHeight="19875" xr2:uid="{D62C98B2-5D28-40CA-95B7-0B218D23B21F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Filename</t>
   </si>
@@ -143,6 +141,9 @@
   </si>
   <si>
     <t>human_GPT_2_80%_feeling so faithless, lost under the surface.txt</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -178,13 +179,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -503,45 +507,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8AC29D-9B7E-457F-B038-A0446CC51115}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Z15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE25" sqref="AE25"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="37" customWidth="1"/>
-    <col min="9" max="9" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="37" customWidth="1"/>
     <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="37" customWidth="1"/>
-    <col min="21" max="21" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="47.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="52.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="59.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -618,104 +622,464 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>3</v>
+      </c>
+      <c r="X8">
+        <v>2.5</v>
+      </c>
+      <c r="Y8">
+        <v>3</v>
+      </c>
+      <c r="Z8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>3</v>
+      </c>
+      <c r="W9">
+        <v>2.5</v>
+      </c>
+      <c r="X9">
+        <v>3</v>
+      </c>
+      <c r="Y9">
+        <v>2.5</v>
+      </c>
+      <c r="Z9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>2.5</v>
+      </c>
+      <c r="W10">
+        <v>3</v>
+      </c>
+      <c r="X10">
+        <v>2.5</v>
+      </c>
+      <c r="Y10">
+        <v>3.5</v>
+      </c>
+      <c r="Z10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="V11">
+        <v>2.5</v>
+      </c>
+      <c r="W11">
+        <v>2.5</v>
+      </c>
+      <c r="X11">
+        <v>3.5</v>
+      </c>
+      <c r="Y11">
+        <v>3.5</v>
+      </c>
+      <c r="Z11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12">
+        <v>3</v>
+      </c>
+      <c r="W12">
+        <v>3</v>
+      </c>
+      <c r="X12">
+        <v>3</v>
+      </c>
+      <c r="Y12">
+        <v>3.5</v>
+      </c>
+      <c r="Z12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -794,8 +1158,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -872,8 +1236,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -950,8 +1314,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1028,8 +1392,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1106,8 +1470,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1186,8 +1550,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1264,8 +1628,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1342,8 +1706,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1420,8 +1784,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1498,13 +1862,526 @@
         <v>2</v>
       </c>
     </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f>AVERAGE(C3,C8,C13,C18,C23)</f>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:Z32" si="0">AVERAGE(D3,D8,D13,D18,D23)</f>
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:R32" si="1">AVERAGE(C4,C9,C14,C19,C24)</f>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="0"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="0"/>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="0"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="0"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A28:A32"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A3:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added my human evaluation
</commit_message>
<xml_diff>
--- a/output/Human Evaluation of Output.xlsx
+++ b/output/Human Evaluation of Output.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ef5aed61654d1d2/School/SMU/Modules/CS605_NLP_for_Smart_Assistants/Project/NLP-Lyric-Generator/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quekh\Desktop\MITB\Academic\CS605 NLP\Group Project\NLP-Lyric-Generator\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{3F379EBD-FB43-8A4D-A37E-DD25ED4CA8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B60CFB2F-F5C6-420F-A94C-9C63F8A048BE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DE072B-32F6-4113-9B1C-E241C776C0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52455" yWindow="720" windowWidth="27045" windowHeight="19875" xr2:uid="{D62C98B2-5D28-40CA-95B7-0B218D23B21F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D62C98B2-5D28-40CA-95B7-0B218D23B21F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Filename</t>
   </si>
@@ -144,6 +146,24 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>human_s2s_lstm_att_long_win-and so this i know.txt</t>
+  </si>
+  <si>
+    <t>human_s2s_lstm_att_long_win-whenever i think back.txt</t>
+  </si>
+  <si>
+    <t>human_s2s_lstm_att_long_win-we will rise stronger together.txt</t>
+  </si>
+  <si>
+    <t>human_s2s_lstm_att_long_win-relight our fire we will find our way.txt</t>
+  </si>
+  <si>
+    <t>human_s2s_lstm_att_long_win-i am tired of being what you want me to be.txt</t>
+  </si>
+  <si>
+    <t>human_s2s_lstm_att_long_win-feeling so faithless lost under the surface.txt</t>
   </si>
 </sst>
 </file>
@@ -188,10 +208,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,45 +527,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8AC29D-9B7E-457F-B038-A0446CC51115}">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="37" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="37" customWidth="1"/>
     <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="37" customWidth="1"/>
-    <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="46.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="49.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="65.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -621,41 +647,509 @@
       <c r="Z2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="AA2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1.5</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1.5</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1.5</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1.5</v>
+      </c>
+      <c r="I4">
+        <v>1.5</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1.5</v>
+      </c>
+      <c r="O4">
+        <v>1.5</v>
+      </c>
+      <c r="P4">
+        <v>1.5</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1.5</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1.5</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>1.5</v>
+      </c>
+      <c r="W4">
+        <v>4</v>
+      </c>
+      <c r="X4">
+        <v>1.5</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>4</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>1.5</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>1.5</v>
+      </c>
+      <c r="AE4">
+        <v>1.5</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1.5</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>3</v>
+      </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1.5</v>
+      </c>
+      <c r="J6">
+        <v>1.5</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1.5</v>
+      </c>
+      <c r="J7">
+        <v>1.5</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>1.5</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="Z7">
+        <v>3</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -734,8 +1228,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -812,8 +1306,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -890,8 +1384,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -968,8 +1462,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1046,40 +1540,40 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1158,8 +1652,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1236,8 +1730,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1314,8 +1808,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1392,8 +1886,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1470,8 +1964,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1550,8 +2044,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1628,8 +2122,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1706,8 +2200,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1784,8 +2278,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1862,8 +2356,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1911,7 +2405,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
@@ -1931,7 +2425,7 @@
       </c>
       <c r="R28">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="S28">
         <f t="shared" si="0"/>
@@ -1943,31 +2437,31 @@
       </c>
       <c r="U28">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
+        <v>3.25</v>
       </c>
       <c r="V28">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>2.75</v>
       </c>
       <c r="W28">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="X28">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2.375</v>
       </c>
       <c r="Y28">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="Z28">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1981,11 +2475,11 @@
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
@@ -1993,15 +2487,15 @@
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="J29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="K29">
         <f t="shared" si="1"/>
@@ -2017,15 +2511,15 @@
       </c>
       <c r="N29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="O29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="P29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="Q29">
         <f t="shared" si="1"/>
@@ -2033,7 +2527,7 @@
       </c>
       <c r="R29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="S29">
         <f t="shared" si="0"/>
@@ -2041,7 +2535,7 @@
       </c>
       <c r="T29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="U29">
         <f t="shared" si="0"/>
@@ -2049,27 +2543,27 @@
       </c>
       <c r="V29">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <v>2.125</v>
       </c>
       <c r="W29">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2.875</v>
       </c>
       <c r="X29">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <v>2.125</v>
       </c>
       <c r="Y29">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2.875</v>
       </c>
       <c r="Z29">
         <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
@@ -2099,11 +2593,11 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
@@ -2147,31 +2641,31 @@
       </c>
       <c r="U30">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
+        <v>3.25</v>
       </c>
       <c r="V30">
         <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
+        <v>1.875</v>
       </c>
       <c r="W30">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <v>2.5</v>
       </c>
       <c r="X30">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.375</v>
       </c>
       <c r="Y30">
         <f t="shared" si="0"/>
-        <v>2.8333333333333335</v>
+        <v>2.875</v>
       </c>
       <c r="Z30">
         <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
@@ -2201,11 +2695,11 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
@@ -2249,31 +2743,31 @@
       </c>
       <c r="U31">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="V31">
         <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
+        <v>1.875</v>
       </c>
       <c r="W31">
         <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
+        <v>1.875</v>
       </c>
       <c r="X31">
         <f t="shared" si="0"/>
-        <v>1.8333333333333333</v>
+        <v>1.625</v>
       </c>
       <c r="Y31">
         <f t="shared" si="0"/>
-        <v>3.1666666666666665</v>
+        <v>2.875</v>
       </c>
       <c r="Z31">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
@@ -2303,11 +2797,11 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="K32">
         <f t="shared" si="0"/>
@@ -2351,27 +2845,27 @@
       </c>
       <c r="U32">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.375</v>
       </c>
       <c r="V32">
         <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <v>2.25</v>
       </c>
       <c r="W32">
         <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
+        <v>2.75</v>
       </c>
       <c r="X32">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="Y32">
         <f t="shared" si="0"/>
-        <v>2.8333333333333335</v>
+        <v>2.875</v>
       </c>
       <c r="Z32">
         <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
+        <v>2.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included evaluation of seq2seq output
</commit_message>
<xml_diff>
--- a/output/Human Evaluation of Output.xlsx
+++ b/output/Human Evaluation of Output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tituslim/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011A0AD8-83BF-45CA-AE48-02CC0825779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E804C0F-EF23-2E43-B331-7E8B2668AE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{D62C98B2-5D28-40CA-95B7-0B218D23B21F}"/>
+    <workbookView xWindow="32980" yWindow="2920" windowWidth="30780" windowHeight="17080" xr2:uid="{D62C98B2-5D28-40CA-95B7-0B218D23B21F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -530,48 +530,48 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AF3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF18" sqref="AF18"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="37" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="37" customWidth="1"/>
     <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="37" customWidth="1"/>
-    <col min="21" max="21" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="47.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="52.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="59.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="57.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="46.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="49.7265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="55.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="60.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="67.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="65.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="59.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="60.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="67.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="65.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -666,7 +666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -1438,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1534,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -1630,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -1824,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -1920,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -2016,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -2191,8 +2191,26 @@
       <c r="Z18">
         <v>3</v>
       </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
@@ -2269,8 +2287,26 @@
       <c r="Z19">
         <v>2</v>
       </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>3</v>
@@ -2347,8 +2383,26 @@
       <c r="Z20">
         <v>2</v>
       </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>1</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -2425,8 +2479,26 @@
       <c r="Z21">
         <v>2</v>
       </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
         <v>5</v>
@@ -2503,8 +2575,26 @@
       <c r="Z22">
         <v>2</v>
       </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22">
+        <v>1</v>
+      </c>
+      <c r="AE22">
+        <v>1</v>
+      </c>
+      <c r="AF22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -2584,7 +2674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>2</v>
@@ -2662,7 +2752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -2740,7 +2830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
@@ -2818,7 +2908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -2896,7 +2986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -3000,7 +3090,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>2</v>
@@ -3102,7 +3192,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
         <v>3</v>
@@ -3204,7 +3294,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="1" t="s">
         <v>4</v>
@@ -3306,7 +3396,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>5</v>

</xml_diff>